<commit_message>
Modified Agile Menifesto Exercise
</commit_message>
<xml_diff>
--- a/M2_SDE_Assignments/cs1_Agile_Manifesto/Agil-Epics-Menifesto.xlsx
+++ b/M2_SDE_Assignments/cs1_Agile_Manifesto/Agil-Epics-Menifesto.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9264" tabRatio="284"/>
+    <workbookView windowWidth="23040" windowHeight="9264" tabRatio="284" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Product Catalog" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="113">
   <si>
     <t>Project Name</t>
   </si>
@@ -204,6 +204,9 @@
     <t>Story Task 1.1: SubTasks</t>
   </si>
   <si>
+    <t>Assignee</t>
+  </si>
+  <si>
     <t>Story Task 1.2: SubTasks</t>
   </si>
   <si>
@@ -213,28 +216,49 @@
     <t>Create wireframes and mockups for the homepage</t>
   </si>
   <si>
+    <t>Designer</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
     <t>Research and draft content about Agile and its origins</t>
   </si>
   <si>
+    <t>QA</t>
+  </si>
+  <si>
     <t>Design a navigation menu with links to other sections</t>
   </si>
   <si>
     <t>Develop HTML and CSS for the homepage layout.</t>
   </si>
   <si>
+    <t>Developer</t>
+  </si>
+  <si>
     <t>Format and add content to the homepage.</t>
   </si>
   <si>
     <t>Implement navigation menu functionality using JavaScript.</t>
   </si>
   <si>
+    <t>Ongoing</t>
+  </si>
+  <si>
     <t>Implement responsive design for mobile and desktop.</t>
   </si>
   <si>
     <t>Ensure the content is concise and visually appealing.</t>
   </si>
   <si>
+    <t>To-Do</t>
+  </si>
+  <si>
     <t>Test navigation links for usability and accessibility</t>
+  </si>
+  <si>
+    <t>Tester</t>
   </si>
   <si>
     <t>Integrate animations for a polished user experience.</t>
@@ -1419,7 +1443,7 @@
   <sheetPr/>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+    <sheetView topLeftCell="D6" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -1904,21 +1928,25 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.8518518518519" defaultRowHeight="24.95" customHeight="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="20.8518518518519" defaultRowHeight="24.95" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="54.2222222222222" style="1" customWidth="1"/>
-    <col min="2" max="2" width="53.8888888888889" style="1" customWidth="1"/>
-    <col min="3" max="3" width="58.1111111111111" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="20.8518518518519" style="1"/>
+    <col min="2" max="2" width="23.7777777777778" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.4444444444444" style="1" customWidth="1"/>
+    <col min="4" max="4" width="53.8888888888889" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.8888888888889" style="1" customWidth="1"/>
+    <col min="7" max="7" width="58.1111111111111" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="20.8518518518519" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:3">
+    <row r="1" customHeight="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>52</v>
       </c>
@@ -1926,203 +1954,499 @@
         <v>53</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" customHeight="1" spans="1:3">
+      <c r="E1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" customHeight="1" spans="1:9">
       <c r="A2" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" customHeight="1" spans="1:3">
+      <c r="I2" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" customHeight="1" spans="1:9">
       <c r="A3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" customHeight="1" spans="1:9">
+      <c r="A4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" customHeight="1" spans="1:9">
+      <c r="A5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" customHeight="1" spans="1:9">
+      <c r="A6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="8" customHeight="1" spans="1:9">
+      <c r="A8" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" customHeight="1" spans="1:9">
+      <c r="A9" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" customHeight="1" spans="1:3">
-      <c r="A4" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="I9" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" customHeight="1" spans="1:9">
+      <c r="A10" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="5" customHeight="1" spans="1:3">
-      <c r="A5" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" customHeight="1" spans="1:3">
-      <c r="A6" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="8" customHeight="1" spans="1:3">
-      <c r="A8" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" customHeight="1" spans="1:3">
-      <c r="A9" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" customHeight="1" spans="1:9">
+      <c r="A11" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="10" customHeight="1" spans="1:3">
-      <c r="A10" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" customHeight="1" spans="1:3">
-      <c r="A11" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" customHeight="1" spans="1:3">
+      <c r="F11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" customHeight="1" spans="1:9">
       <c r="A13" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" customHeight="1" spans="1:3">
+        <v>86</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" customHeight="1" spans="1:9">
       <c r="A14" s="3" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" customHeight="1" spans="1:3">
+        <v>69</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" customHeight="1" spans="1:9">
       <c r="A15" s="3" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" customHeight="1" spans="1:3">
+        <v>69</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" customHeight="1" spans="1:9">
       <c r="A16" s="3" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" customHeight="1" spans="1:3">
+        <v>69</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" customHeight="1" spans="1:9">
       <c r="A18" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" customHeight="1" spans="1:3">
+        <v>98</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" customHeight="1" spans="1:9">
       <c r="A19" s="3" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" customHeight="1" spans="1:3">
+        <v>69</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" customHeight="1" spans="1:9">
       <c r="A20" s="3" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" customHeight="1" spans="1:3">
+        <v>69</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" customHeight="1" spans="1:9">
       <c r="A21" s="3" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" customHeight="1" spans="1:3">
+        <v>69</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" customHeight="1" spans="1:9">
       <c r="A22" s="3" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" customHeight="1" spans="1:3">
+        <v>63</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" customHeight="1" spans="1:9">
       <c r="A23" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
+        <v>112</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>